<commit_message>
mostly working with seedling plot AICc analysis
</commit_message>
<xml_diff>
--- a/Figures and Graphs/figures/revised scat table.xlsx
+++ b/Figures and Graphs/figures/revised scat table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t> </t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>unknown*</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +142,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,26 +204,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -615,9 +600,8 @@
       <c r="C3" s="11">
         <v>0</v>
       </c>
-      <c r="D3" s="11">
-        <f>B3/20</f>
-        <v>0</v>
+      <c r="D3" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="11">
         <v>1119</v>
@@ -626,8 +610,8 @@
         <v>20</v>
       </c>
       <c r="G3" s="12">
-        <f>E3/31</f>
-        <v>36.096774193548384</v>
+        <f>E3/F3</f>
+        <v>55.95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -640,9 +624,8 @@
       <c r="C4" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
-        <f t="shared" ref="D4:D12" si="0">B4/20</f>
-        <v>0</v>
+      <c r="D4" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="E4" s="11">
         <v>247</v>
@@ -651,8 +634,8 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ref="G4:G12" si="1">E4/31</f>
-        <v>7.967741935483871</v>
+        <f t="shared" ref="G4:G12" si="0">E4/F4</f>
+        <v>82.333333333333329</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -665,9 +648,9 @@
       <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="14">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+      <c r="D5" s="11">
+        <f t="shared" ref="D4:D12" si="1">B5/C5</f>
+        <v>1</v>
       </c>
       <c r="E5" s="13">
         <v>266</v>
@@ -675,9 +658,9 @@
       <c r="F5" s="13">
         <v>16</v>
       </c>
-      <c r="G5" s="15">
-        <f t="shared" si="1"/>
-        <v>8.5806451612903221</v>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>16.625</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -690,9 +673,9 @@
       <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="14">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+      <c r="D6" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
@@ -700,9 +683,8 @@
       <c r="F6" s="13">
         <v>0</v>
       </c>
-      <c r="G6" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G6" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -715,9 +697,9 @@
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="14">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
+      <c r="D7" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="E7" s="13">
         <v>13</v>
@@ -725,9 +707,9 @@
       <c r="F7" s="13">
         <v>3</v>
       </c>
-      <c r="G7" s="15">
-        <f t="shared" si="1"/>
-        <v>0.41935483870967744</v>
+      <c r="G7" s="12">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -740,9 +722,9 @@
       <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="14">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+      <c r="D8" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
@@ -750,9 +732,8 @@
       <c r="F8" s="13">
         <v>0</v>
       </c>
-      <c r="G8" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G8" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -765,9 +746,8 @@
       <c r="C9" s="13">
         <v>0</v>
       </c>
-      <c r="D9" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D9" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
@@ -775,9 +755,9 @@
       <c r="F9" s="13">
         <v>3</v>
       </c>
-      <c r="G9" s="15">
-        <f t="shared" si="1"/>
-        <v>9.6774193548387094E-2</v>
+      <c r="G9" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -790,19 +770,18 @@
       <c r="C10" s="13">
         <v>0</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" si="1"/>
-        <v>3.2258064516129031E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -815,44 +794,43 @@
       <c r="C11" s="13">
         <v>0</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="13">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15">
-        <f t="shared" si="1"/>
-        <v>3.2258064516129031E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>2</v>
       </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17">
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>8</v>
+      </c>
+      <c r="F12" s="14">
+        <v>4</v>
+      </c>
+      <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="16">
-        <v>8</v>
-      </c>
-      <c r="F12" s="16">
-        <v>4</v>
-      </c>
-      <c r="G12" s="18">
-        <f t="shared" si="1"/>
-        <v>0.25806451612903225</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -872,7 +850,7 @@
       <c r="F13" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>